<commit_message>
minimax and combat modeling
</commit_message>
<xml_diff>
--- a/WestPoint/Combat Modelling/4,5HW- Shooting, Comunication and Target Acquisition.xlsx
+++ b/WestPoint/Combat Modelling/4,5HW- Shooting, Comunication and Target Acquisition.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usarmywestpoint-my.sharepoint.com/personal/mayara_mendonca_westpoint_edu/Documents/Documents/GitHub/Comp-IME-23/WestPoint/Combat Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="8_{F6007C2C-C2C1-47AA-A4A9-F03125BB31B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8126A9E-2231-45EC-83E9-CC45F0672759}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="8_{F6007C2C-C2C1-47AA-A4A9-F03125BB31B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{521B34E6-C50A-4908-A29E-CD2F9609A28E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{D4C5DF6D-7289-43C6-88B5-F695DB62A401}"/>
+    <workbookView minimized="1" xWindow="3940" yWindow="3490" windowWidth="14400" windowHeight="7270" activeTab="3" xr2:uid="{D4C5DF6D-7289-43C6-88B5-F695DB62A401}"/>
   </bookViews>
   <sheets>
-    <sheet name="Comunication" sheetId="1" r:id="rId1"/>
+    <sheet name="Movement+Comunication" sheetId="1" r:id="rId1"/>
     <sheet name="HW7" sheetId="2" r:id="rId2"/>
     <sheet name="Class24AUG" sheetId="4" r:id="rId3"/>
     <sheet name="Class26AUG" sheetId="5" r:id="rId4"/>
@@ -301,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -320,9 +320,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1864,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CE9E27-4C85-4D29-985D-C2C55F42F9B0}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2042,7 +2039,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3242,7 +3239,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3413,8 +3410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A5CD9C-E437-4254-BFAC-78492E8861DE}">
   <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3471,15 +3468,15 @@
       <c r="S1" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>65</v>
       </c>
       <c r="V1" s="6"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2">
@@ -3779,7 +3776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714BEC97-0B24-4922-AC07-00DD386316BF}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>

</xml_diff>